<commit_message>
Update List of MegaMod and Firmware.xlsx
</commit_message>
<xml_diff>
--- a/List of MegaMod and Firmware.xlsx
+++ b/List of MegaMod and Firmware.xlsx
@@ -609,7 +609,7 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -664,7 +664,7 @@
         <v>9</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>56</v>
@@ -687,7 +687,7 @@
         <v>9</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>12</v>

</xml_diff>